<commit_message>
Added refresh functionality and added scroll bar, bill storage fun
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">ImagePath</t>
   </si>
   <si>
-    <t xml:space="preserve">Vada Pav</t>
+    <t xml:space="preserve">वडापाव</t>
   </si>
   <si>
     <t xml:space="preserve">images/vadapav.avif</t>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t xml:space="preserve">images/cold.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cake 500g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cake 1000g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurkure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pani bottle Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pani Bottle Mothi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchurian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misal Pav</t>
   </si>
 </sst>
 </file>
@@ -80,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -110,6 +134,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,6 +194,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -184,15 +218,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -277,13 +312,104 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="वडापाव"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>